<commit_message>
fix(data): Cap QA data to 5 paragraphs, 20 Qs
Cap the question-answering dataset to 5 paragraphs per article, to
avoid exceeding context limits on more SM JumpStart models and to
improve presentation of interfaces e.g. in Streamlit and human eval
jobs. Also limit the dataset from 35 to 20 total questions/articles,
to speed up manual labelling lab.
</commit_message>
<xml_diff>
--- a/datasets/question-answering/qa.xlsx
+++ b/datasets/question-answering/qa.xlsx
@@ -125,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbl_annotations" displayName="tbl_annotations" ref="A1:C36" headerRowCount="1">
-  <autoFilter ref="A1:C36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbl_annotations" displayName="tbl_annotations" ref="A1:C21" headerRowCount="1">
+  <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Question"/>
     <tableColumn id="2" name="Reference Answer(s)"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,261 +790,6 @@
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>What individual is the school named after?</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>John Harvard</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Harvard_University</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Which Florida city has the biggest population?</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Jacksonville</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Jacksonville,_Florida</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>What percentage of global assets does the richest 1% of people have?</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>40%&lt;OR&gt;40</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Economic_inequality</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>What kind of university is the University of Chicago?</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>a private research university&lt;OR&gt;private research&lt;OR&gt;private research university</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>University_of_Chicago</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>What is the Chinese name for the Yuan dynasty?</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Yuán Cháo&lt;OR&gt;元朝</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Yuan_dynasty</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>The immune system protects organisms against what?</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>disease</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Immune_system</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>What organization is the IPCC a part of?</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>the United Nations</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Intergovernmental_Panel_on_Climate_Change</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>What is the only divisor besides 1 that a prime number can have?</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>itself</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Prime_number</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Where does the Rhine empty?</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>North Sea&lt;OR&gt;the North Sea in the Netherlands</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Rhine</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>When was the current parliament of Scotland convened?</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Following a referendum in 1997&lt;OR&gt;1998</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Scottish_Parliament</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>What is an Islamic revival movement?</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Islamism</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Islamism</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The word imperialism has it's origins in which ancient language? </t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Latin</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Imperialism</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>What is the largest city of Poland?</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Warsaw</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Warsaw</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>When was the French and Indian War?</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>1754–1763</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>French_and_Indian_War</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>What concept did philosophers in antiquity use to study simple machines?</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>force&lt;OR&gt;the concept of force</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Force</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>